<commit_message>
Update SVI to be rplthemes (overall measure); add table 4 to report. Now have comparison of no policy/policy and 75th percentile cutoff.
</commit_message>
<xml_diff>
--- a/construct_texts.xlsx
+++ b/construct_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/53643/Library/CloudStorage/OneDrive-ICF/Work/work_2022/nscps_district_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55755FA7-DCEF-8440-BCCD-D6E0660F9214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BF971B-30FE-7A42-A80E-3C1F10D41394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16100" yWindow="2180" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
   <si>
     <t>construct</t>
   </si>
@@ -85,18 +85,6 @@
     <t>percentstudentsfreereducedlunch</t>
   </si>
   <si>
-    <t>rpltheme1</t>
-  </si>
-  <si>
-    <t>rpltheme2</t>
-  </si>
-  <si>
-    <t>rpltheme3</t>
-  </si>
-  <si>
-    <t>rpltheme4</t>
-  </si>
-  <si>
     <t>rplthemes</t>
   </si>
   <si>
@@ -343,7 +331,40 @@
     <t>75th percentile Cohorting and/or staggering policy</t>
   </si>
   <si>
-    <t>vaccination\\.50</t>
+    <t>vaccinationquarter.nonzero</t>
+  </si>
+  <si>
+    <t>etiquettequarter.nonzero</t>
+  </si>
+  <si>
+    <t>masksquarter.nonzero</t>
+  </si>
+  <si>
+    <t>physicaldistancingquarter.nonzero</t>
+  </si>
+  <si>
+    <t>cohortingorstaggeringquarter.nonzero</t>
+  </si>
+  <si>
+    <t>testingandscreeningquarter.nonzero</t>
+  </si>
+  <si>
+    <t>stayhomequarter.nonzero</t>
+  </si>
+  <si>
+    <t>traceandquarantinequarter.nonzero</t>
+  </si>
+  <si>
+    <t>cleaningquarter.nonzero</t>
+  </si>
+  <si>
+    <t>ventilationquarter.nonzero</t>
+  </si>
+  <si>
+    <t>vaccination.50</t>
+  </si>
+  <si>
+    <t>SVI Overall Rank</t>
   </si>
 </sst>
 </file>
@@ -730,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -747,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -755,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -763,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -771,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -779,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -787,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -795,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -803,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -811,7 +832,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -819,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -827,7 +848,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -835,7 +856,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -843,7 +864,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -851,7 +872,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -859,7 +880,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -867,7 +888,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -875,7 +896,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -883,7 +904,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -891,7 +912,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -899,7 +920,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -907,37 +928,52 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>86</v>
@@ -996,7 +1032,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1004,7 +1040,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1012,7 +1048,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1020,7 +1056,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1028,7 +1064,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1036,7 +1072,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1068,7 +1104,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1076,7 +1112,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1084,7 +1120,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1092,7 +1128,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1100,7 +1136,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1108,7 +1144,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1116,7 +1152,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1132,7 +1168,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1148,7 +1184,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1156,7 +1192,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1164,7 +1200,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1172,7 +1208,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1180,7 +1216,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1188,7 +1224,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1196,7 +1232,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1204,7 +1240,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1212,7 +1248,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1220,39 +1256,87 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" t="s">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
-        <v>72</v>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing rough draft of manuscript/report. Realized free and reduce lunch missing more than was before, so replaced missing with stats from 2019-20 when available from NCES. Did this for race variables as well.
</commit_message>
<xml_diff>
--- a/construct_texts.xlsx
+++ b/construct_texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/53643_icf_com/Documents/Work/work_2022/nscps_district_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{D2BF971B-30FE-7A42-A80E-3C1F10D41394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E89E0EF-42CF-D344-8547-DEC0DEDB0569}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{D2BF971B-30FE-7A42-A80E-3C1F10D41394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43152B3C-1D9F-EC40-8CEB-1A0D59FB8B2E}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="1900" windowWidth="20060" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20960" yWindow="1900" windowWidth="13600" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>construct</t>
   </si>
@@ -172,10 +172,52 @@
     <t>Intercept</t>
   </si>
   <si>
-    <t>percentfreelunchqualified</t>
-  </si>
-  <si>
-    <t>Percent free lunch qualified</t>
+    <t>ss1</t>
+  </si>
+  <si>
+    <t>ss2</t>
+  </si>
+  <si>
+    <t>ss3</t>
+  </si>
+  <si>
+    <t>ss4</t>
+  </si>
+  <si>
+    <t>ss5</t>
+  </si>
+  <si>
+    <t>One strategy</t>
+  </si>
+  <si>
+    <t>Two strategies</t>
+  </si>
+  <si>
+    <t>Three strategies</t>
+  </si>
+  <si>
+    <t>Four strategies</t>
+  </si>
+  <si>
+    <t>Five strategies</t>
+  </si>
+  <si>
+    <t>schoollevelHS</t>
+  </si>
+  <si>
+    <t>schoollevelMS</t>
+  </si>
+  <si>
+    <t>High school</t>
+  </si>
+  <si>
+    <t>Middle school</t>
+  </si>
+  <si>
+    <t>Percent free and reduced lunch</t>
+  </si>
+  <si>
+    <t>percentfreereducedlunch</t>
   </si>
 </sst>
 </file>
@@ -566,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,10 +782,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -784,6 +826,62 @@
       </c>
       <c r="B26" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added discussion and new script, 07 that analyses outcomes using multiple cumulative indices. these are put into the final table of results.
</commit_message>
<xml_diff>
--- a/construct_texts.xlsx
+++ b/construct_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/53643_icf_com/Documents/Work/work_2022/nscps_district_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{D2BF971B-30FE-7A42-A80E-3C1F10D41394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43152B3C-1D9F-EC40-8CEB-1A0D59FB8B2E}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{D2BF971B-30FE-7A42-A80E-3C1F10D41394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A5EFAE7-CFBC-1249-95B6-96069808FDDA}"/>
   <bookViews>
     <workbookView xWindow="20960" yWindow="1900" windowWidth="13600" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>construct</t>
   </si>
@@ -187,21 +187,6 @@
     <t>ss5</t>
   </si>
   <si>
-    <t>One strategy</t>
-  </si>
-  <si>
-    <t>Two strategies</t>
-  </si>
-  <si>
-    <t>Three strategies</t>
-  </si>
-  <si>
-    <t>Four strategies</t>
-  </si>
-  <si>
-    <t>Five strategies</t>
-  </si>
-  <si>
     <t>schoollevelHS</t>
   </si>
   <si>
@@ -218,6 +203,18 @@
   </si>
   <si>
     <t>percentfreereducedlunch</t>
+  </si>
+  <si>
+    <t>ss6</t>
+  </si>
+  <si>
+    <t>ss7</t>
+  </si>
+  <si>
+    <t>ss8</t>
+  </si>
+  <si>
+    <t>ss9</t>
   </si>
 </sst>
 </file>
@@ -608,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -782,10 +779,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -832,56 +829,88 @@
       <c r="A27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
-        <v>55</v>
+      <c r="B27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
-        <v>56</v>
+      <c r="B28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
-        <v>57</v>
+      <c r="B29">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
-        <v>58</v>
+      <c r="B30">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
-      <c r="B31" t="s">
-        <v>59</v>
+      <c r="B31">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>63</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>